<commit_message>
Adding cronbachs alpha analysis
</commit_message>
<xml_diff>
--- a/Data/processed/Flow_endo_post_3_002_2019_Mar_27_1845.xlsx
+++ b/Data/processed/Flow_endo_post_3_002_2019_Mar_27_1845.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manfred Mustermann\OneDrive\Dokumente\Science\Analysevorbereitungen\flow_raw_data\processed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manfred Mustermann\OneDrive\Dokumente\Science\Scotts lab\Flow_states_and_Spatiotemporal_Processing\Data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB49DBC0-CE18-4BD1-AD57-36BE20A80CA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{DB49DBC0-CE18-4BD1-AD57-36BE20A80CA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D2422F15-BA6C-49FD-A715-40F417253763}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="615" windowWidth="28755" windowHeight="15585" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow_endo_post_3_002_2019_Mar_2" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,17 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -268,7 +278,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1102,14 +1112,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN142"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="AC127" sqref="AC127"/>
+    <sheetView topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="P142" sqref="A117:P142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -8023,7 +8039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15120,7 +15136,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16731,11 +16747,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AB27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB27" sqref="AB27"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>